<commit_message>
vitalclinic folder updated 19 10 24
</commit_message>
<xml_diff>
--- a/inventario de equipos en caja.xlsx
+++ b/inventario de equipos en caja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguelr\Desktop\TRABAJO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7398D20F-16F5-4543-8DDD-326E0AD71FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAA7AD3-C1B0-4338-9A9C-8A31BF2989C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{F0B0A52F-C4CA-4303-BB1F-3D41201E624C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>descripcion</t>
   </si>
@@ -228,13 +228,106 @@
   </si>
   <si>
     <t>CABLE ETHERNET PONCHADO RJ45 3+ mts</t>
+  </si>
+  <si>
+    <t>DVR de 16 Canales Dahua Penta-Brid 1080N,720p,Compacto 1U, H.265,1HDD 6Tb WizSense ,Ancho de banda 64 Mbps</t>
+  </si>
+  <si>
+    <t>DVR DE CAMARAS 
+DE VIGILANCIA</t>
+  </si>
+  <si>
+    <t>DH-XVR1B16</t>
+  </si>
+  <si>
+    <t>ALHUA</t>
+  </si>
+  <si>
+    <t>TRAE SU PROPIO 
+CABLE DE CARGA</t>
+  </si>
+  <si>
+    <t>nº SERIE</t>
+  </si>
+  <si>
+    <t>5K0978BPAZ9D6D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIGITAL VIDEO RECORDER iDS-7216HQHI-M2-S
+16-ch 1080p 1U H.265 AcuSense </t>
+  </si>
+  <si>
+    <t>DVR</t>
+  </si>
+  <si>
+    <t>iDS-7216HQHI-M2-S</t>
+  </si>
+  <si>
+    <t>HIKVISION</t>
+  </si>
+  <si>
+    <t>G35112958</t>
+  </si>
+  <si>
+    <t>HILOOK COLOR CAMERA</t>
+  </si>
+  <si>
+    <t>CAMARA DE 
+VIGILANCIA</t>
+  </si>
+  <si>
+    <t>THC-T129-P
+ 2.8MM</t>
+  </si>
+  <si>
+    <t>G81033739</t>
+  </si>
+  <si>
+    <t>THC-T129-M
+ 2.8MM</t>
+  </si>
+  <si>
+    <t>G81006961</t>
+  </si>
+  <si>
+    <t>CAMARA COLOR HIKVISION</t>
+  </si>
+  <si>
+    <t>DS-2CE56D0T-IRMMF
+2,8MM</t>
+  </si>
+  <si>
+    <t>D14627441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDCVI CAMERA </t>
+  </si>
+  <si>
+    <t>DH-HAC-T1A21N</t>
+  </si>
+  <si>
+    <t>5K0509BPAR32963</t>
+  </si>
+  <si>
+    <t>BASES PARA CAMARA HIKVISION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONECTORES DE ENERGIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAEN SU ADAPTADOR 
+ DE  CORRIENTE Y
+ DE SEÑAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +354,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF656565"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -296,6 +404,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F05098A-E9E7-487F-B712-509FA6460BAE}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +744,7 @@
     <col min="6" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,8 +763,11 @@
       <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -662,7 +783,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -680,7 +801,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -698,7 +819,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -714,7 +835,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
@@ -732,7 +853,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -750,7 +871,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -766,7 +887,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -780,7 +901,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -796,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -806,7 +927,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -820,7 +941,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -832,7 +953,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -846,7 +967,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -860,7 +981,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -870,7 +991,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -886,7 +1007,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -896,7 +1017,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -906,7 +1027,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -920,7 +1041,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -930,7 +1051,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
@@ -940,7 +1061,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -948,37 +1069,147 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+    <row r="24" spans="1:7" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="G25" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="3">
+        <v>9</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>